<commit_message>
File Decoder Model fixed, need to add db for it
</commit_message>
<xml_diff>
--- a/src/main/java/excel_decoder_files/sm_decoder_file.xlsx
+++ b/src/main/java/excel_decoder_files/sm_decoder_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\LaborDashboard\src\main\java\excel_decoder_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D92094-64C3-42EF-9B9C-8E66C93804FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC74F27-E82C-4C63-9851-D7476B2D6FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11625" yWindow="0" windowWidth="17175" windowHeight="15600" activeTab="1" xr2:uid="{BF93DD93-9419-4F7C-BCB7-368AC606ADC2}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{BF93DD93-9419-4F7C-BCB7-368AC606ADC2}"/>
   </bookViews>
   <sheets>
     <sheet name="Series ID Format" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="920">
   <si>
     <t>state_code</t>
   </si>
@@ -2770,6 +2770,33 @@
   </si>
   <si>
     <t>Securities Brokerage</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>00000</t>
   </si>
 </sst>
 </file>
@@ -3359,14 +3386,13 @@
   <dimension ref="A1:P449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="13" customWidth="1"/>
-    <col min="4" max="6" width="18.85546875" style="12" customWidth="1"/>
+    <col min="3" max="6" width="18.85546875" style="12" customWidth="1"/>
     <col min="7" max="7" width="18.85546875" style="13" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" style="12" customWidth="1"/>
     <col min="9" max="10" width="18.85546875" style="10" customWidth="1"/>
@@ -3419,14 +3445,14 @@
       <c r="B2" t="s">
         <v>880</v>
       </c>
-      <c r="C2" s="8">
-        <v>0</v>
+      <c r="C2" s="10" t="s">
+        <v>918</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10">
-        <v>0</v>
+      <c r="E2" s="10" t="s">
+        <v>919</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>10</v>
@@ -3458,8 +3484,8 @@
       <c r="B3" t="s">
         <v>881</v>
       </c>
-      <c r="C3" s="8">
-        <v>1</v>
+      <c r="C3" s="10" t="s">
+        <v>911</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>12</v>
@@ -3490,8 +3516,8 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="54">
-      <c r="C4" s="8">
-        <v>2</v>
+      <c r="C4" s="10" t="s">
+        <v>912</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>15</v>
@@ -3522,8 +3548,8 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="54">
-      <c r="C5" s="8">
-        <v>4</v>
+      <c r="C5" s="10" t="s">
+        <v>913</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>18</v>
@@ -3554,8 +3580,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="54">
-      <c r="C6" s="8">
-        <v>5</v>
+      <c r="C6" s="10" t="s">
+        <v>914</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>21</v>
@@ -3586,8 +3612,8 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="67.5">
-      <c r="C7" s="8">
-        <v>6</v>
+      <c r="C7" s="10" t="s">
+        <v>915</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>24</v>
@@ -3618,8 +3644,8 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="54">
-      <c r="C8" s="8">
-        <v>8</v>
+      <c r="C8" s="10" t="s">
+        <v>916</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>27</v>
@@ -3650,8 +3676,8 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="81">
-      <c r="C9" s="8">
-        <v>9</v>
+      <c r="C9" s="10" t="s">
+        <v>917</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>31</v>
@@ -3682,7 +3708,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" ht="81">
-      <c r="C10" s="8">
+      <c r="C10" s="10">
         <v>10</v>
       </c>
       <c r="D10" s="9" t="s">
@@ -3714,7 +3740,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" ht="81">
-      <c r="C11" s="8">
+      <c r="C11" s="10">
         <v>11</v>
       </c>
       <c r="D11" s="9" t="s">
@@ -3746,7 +3772,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="81">
-      <c r="C12" s="8">
+      <c r="C12" s="10">
         <v>12</v>
       </c>
       <c r="D12" s="9" t="s">
@@ -3778,7 +3804,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="81">
-      <c r="C13" s="8">
+      <c r="C13" s="10">
         <v>13</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -3810,7 +3836,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" ht="67.5">
-      <c r="C14" s="8">
+      <c r="C14" s="10">
         <v>15</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -3842,7 +3868,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" ht="54">
-      <c r="C15" s="8">
+      <c r="C15" s="10">
         <v>16</v>
       </c>
       <c r="D15" s="9" t="s">
@@ -3869,7 +3895,7 @@
       <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="54">
-      <c r="C16" s="8">
+      <c r="C16" s="10">
         <v>17</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -3895,7 +3921,7 @@
       </c>
     </row>
     <row r="17" spans="3:10" ht="40.5">
-      <c r="C17" s="8">
+      <c r="C17" s="10">
         <v>18</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -3921,7 +3947,7 @@
       </c>
     </row>
     <row r="18" spans="3:10" ht="40.5">
-      <c r="C18" s="8">
+      <c r="C18" s="10">
         <v>19</v>
       </c>
       <c r="D18" s="9" t="s">
@@ -3947,7 +3973,7 @@
       </c>
     </row>
     <row r="19" spans="3:10" ht="40.5">
-      <c r="C19" s="8">
+      <c r="C19" s="10">
         <v>20</v>
       </c>
       <c r="D19" s="9" t="s">
@@ -3973,7 +3999,7 @@
       </c>
     </row>
     <row r="20" spans="3:10" ht="40.5">
-      <c r="C20" s="8">
+      <c r="C20" s="10">
         <v>21</v>
       </c>
       <c r="D20" s="9" t="s">
@@ -3999,7 +4025,7 @@
       </c>
     </row>
     <row r="21" spans="3:10" ht="40.5">
-      <c r="C21" s="8">
+      <c r="C21" s="10">
         <v>22</v>
       </c>
       <c r="D21" s="9" t="s">
@@ -4025,7 +4051,7 @@
       </c>
     </row>
     <row r="22" spans="3:10" ht="40.5">
-      <c r="C22" s="8">
+      <c r="C22" s="10">
         <v>23</v>
       </c>
       <c r="D22" s="9" t="s">
@@ -4051,7 +4077,7 @@
       </c>
     </row>
     <row r="23" spans="3:10" ht="40.5">
-      <c r="C23" s="8">
+      <c r="C23" s="10">
         <v>24</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -4077,7 +4103,7 @@
       </c>
     </row>
     <row r="24" spans="3:10" ht="27">
-      <c r="C24" s="8">
+      <c r="C24" s="10">
         <v>25</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -4098,7 +4124,7 @@
       </c>
     </row>
     <row r="25" spans="3:10" ht="54">
-      <c r="C25" s="8">
+      <c r="C25" s="10">
         <v>26</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -4118,7 +4144,7 @@
       </c>
     </row>
     <row r="26" spans="3:10" ht="54">
-      <c r="C26" s="8">
+      <c r="C26" s="10">
         <v>27</v>
       </c>
       <c r="D26" s="9" t="s">
@@ -4138,7 +4164,7 @@
       </c>
     </row>
     <row r="27" spans="3:10" ht="27">
-      <c r="C27" s="8">
+      <c r="C27" s="10">
         <v>28</v>
       </c>
       <c r="D27" s="9" t="s">
@@ -4158,7 +4184,7 @@
       </c>
     </row>
     <row r="28" spans="3:10" ht="67.5">
-      <c r="C28" s="8">
+      <c r="C28" s="10">
         <v>29</v>
       </c>
       <c r="D28" s="9" t="s">
@@ -4178,7 +4204,7 @@
       </c>
     </row>
     <row r="29" spans="3:10" ht="40.5">
-      <c r="C29" s="8">
+      <c r="C29" s="10">
         <v>30</v>
       </c>
       <c r="D29" s="9" t="s">
@@ -4198,7 +4224,7 @@
       </c>
     </row>
     <row r="30" spans="3:10" ht="40.5">
-      <c r="C30" s="8">
+      <c r="C30" s="10">
         <v>31</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -4218,7 +4244,7 @@
       </c>
     </row>
     <row r="31" spans="3:10" ht="40.5">
-      <c r="C31" s="8">
+      <c r="C31" s="10">
         <v>32</v>
       </c>
       <c r="D31" s="9" t="s">
@@ -4238,7 +4264,7 @@
       </c>
     </row>
     <row r="32" spans="3:10">
-      <c r="C32" s="8">
+      <c r="C32" s="10">
         <v>33</v>
       </c>
       <c r="D32" s="9" t="s">
@@ -4258,7 +4284,7 @@
       </c>
     </row>
     <row r="33" spans="3:10" ht="27">
-      <c r="C33" s="8">
+      <c r="C33" s="10">
         <v>34</v>
       </c>
       <c r="D33" s="9" t="s">
@@ -4278,7 +4304,7 @@
       </c>
     </row>
     <row r="34" spans="3:10" ht="27">
-      <c r="C34" s="8">
+      <c r="C34" s="10">
         <v>35</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -4298,7 +4324,7 @@
       </c>
     </row>
     <row r="35" spans="3:10" ht="40.5">
-      <c r="C35" s="8">
+      <c r="C35" s="10">
         <v>36</v>
       </c>
       <c r="D35" s="9" t="s">
@@ -4318,7 +4344,7 @@
       </c>
     </row>
     <row r="36" spans="3:10" ht="67.5">
-      <c r="C36" s="8">
+      <c r="C36" s="10">
         <v>37</v>
       </c>
       <c r="D36" s="9" t="s">
@@ -4338,7 +4364,7 @@
       </c>
     </row>
     <row r="37" spans="3:10" ht="40.5">
-      <c r="C37" s="8">
+      <c r="C37" s="10">
         <v>38</v>
       </c>
       <c r="D37" s="9" t="s">
@@ -4358,7 +4384,7 @@
       </c>
     </row>
     <row r="38" spans="3:10" ht="40.5">
-      <c r="C38" s="8">
+      <c r="C38" s="10">
         <v>39</v>
       </c>
       <c r="D38" s="9" t="s">
@@ -4378,7 +4404,7 @@
       </c>
     </row>
     <row r="39" spans="3:10" ht="54">
-      <c r="C39" s="8">
+      <c r="C39" s="10">
         <v>40</v>
       </c>
       <c r="D39" s="9" t="s">
@@ -4398,7 +4424,7 @@
       </c>
     </row>
     <row r="40" spans="3:10" ht="27">
-      <c r="C40" s="8">
+      <c r="C40" s="10">
         <v>41</v>
       </c>
       <c r="D40" s="9" t="s">
@@ -4418,7 +4444,7 @@
       </c>
     </row>
     <row r="41" spans="3:10" ht="54">
-      <c r="C41" s="8">
+      <c r="C41" s="10">
         <v>42</v>
       </c>
       <c r="D41" s="9" t="s">
@@ -4438,7 +4464,7 @@
       </c>
     </row>
     <row r="42" spans="3:10">
-      <c r="C42" s="8">
+      <c r="C42" s="10">
         <v>44</v>
       </c>
       <c r="D42" s="9" t="s">
@@ -4458,7 +4484,7 @@
       </c>
     </row>
     <row r="43" spans="3:10" ht="40.5">
-      <c r="C43" s="8">
+      <c r="C43" s="10">
         <v>45</v>
       </c>
       <c r="D43" s="9" t="s">
@@ -4478,7 +4504,7 @@
       </c>
     </row>
     <row r="44" spans="3:10" ht="54">
-      <c r="C44" s="8">
+      <c r="C44" s="10">
         <v>46</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -4498,7 +4524,7 @@
       </c>
     </row>
     <row r="45" spans="3:10" ht="67.5">
-      <c r="C45" s="8">
+      <c r="C45" s="10">
         <v>47</v>
       </c>
       <c r="D45" s="9" t="s">
@@ -4518,7 +4544,7 @@
       </c>
     </row>
     <row r="46" spans="3:10" ht="54">
-      <c r="C46" s="8">
+      <c r="C46" s="10">
         <v>48</v>
       </c>
       <c r="D46" s="9" t="s">
@@ -4538,7 +4564,7 @@
       </c>
     </row>
     <row r="47" spans="3:10" ht="27">
-      <c r="C47" s="8">
+      <c r="C47" s="10">
         <v>49</v>
       </c>
       <c r="D47" s="9" t="s">
@@ -4558,7 +4584,7 @@
       </c>
     </row>
     <row r="48" spans="3:10" ht="67.5">
-      <c r="C48" s="8">
+      <c r="C48" s="10">
         <v>50</v>
       </c>
       <c r="D48" s="9" t="s">
@@ -4578,7 +4604,7 @@
       </c>
     </row>
     <row r="49" spans="3:10" ht="40.5">
-      <c r="C49" s="8">
+      <c r="C49" s="10">
         <v>51</v>
       </c>
       <c r="D49" s="9" t="s">
@@ -4598,7 +4624,7 @@
       </c>
     </row>
     <row r="50" spans="3:10" ht="67.5">
-      <c r="C50" s="8">
+      <c r="C50" s="10">
         <v>53</v>
       </c>
       <c r="D50" s="9" t="s">
@@ -4618,7 +4644,7 @@
       </c>
     </row>
     <row r="51" spans="3:10" ht="54">
-      <c r="C51" s="8">
+      <c r="C51" s="10">
         <v>54</v>
       </c>
       <c r="D51" s="9" t="s">
@@ -4638,7 +4664,7 @@
       </c>
     </row>
     <row r="52" spans="3:10" ht="81">
-      <c r="C52" s="8">
+      <c r="C52" s="10">
         <v>55</v>
       </c>
       <c r="D52" s="9" t="s">
@@ -4658,7 +4684,7 @@
       </c>
     </row>
     <row r="53" spans="3:10" ht="54">
-      <c r="C53" s="8">
+      <c r="C53" s="10">
         <v>56</v>
       </c>
       <c r="D53" s="9" t="s">
@@ -4678,7 +4704,7 @@
       </c>
     </row>
     <row r="54" spans="3:10" ht="54">
-      <c r="C54" s="8">
+      <c r="C54" s="10">
         <v>72</v>
       </c>
       <c r="D54" s="9" t="s">
@@ -4698,7 +4724,7 @@
       </c>
     </row>
     <row r="55" spans="3:10" ht="54">
-      <c r="C55" s="8">
+      <c r="C55" s="10">
         <v>78</v>
       </c>
       <c r="D55" s="9" t="s">
@@ -4718,7 +4744,7 @@
       </c>
     </row>
     <row r="56" spans="3:10" ht="54">
-      <c r="C56" s="8">
+      <c r="C56" s="10">
         <v>99</v>
       </c>
       <c r="D56" s="9" t="s">

</xml_diff>